<commit_message>
fix header template cetak
fix header template cetak
</commit_message>
<xml_diff>
--- a/api/client/templates/cetak/laporan_pemeliharaan_telaah.xlsx
+++ b/api/client/templates/cetak/laporan_pemeliharaan_telaah.xlsx
@@ -44,9 +44,6 @@
     <t>BPPKAD</t>
   </si>
   <si>
-    <t>KUASA PENGGUNA BARANG</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>NAMA PEMELIHARAAN</t>
+  </si>
+  <si>
+    <t>PENGGUNA BARANG</t>
   </si>
 </sst>
 </file>
@@ -253,17 +253,38 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,27 +297,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +581,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+      <selection activeCell="A4" sqref="A4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,76 +595,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -683,11 +683,11 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -701,11 +701,11 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -719,9 +719,9 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -745,130 +745,125 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="17"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="6">
         <v>1</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="6">
         <v>6</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="6">
         <v>7</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="6">
         <v>8</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="6">
         <v>9</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="6">
         <v>10</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="6">
         <v>11</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="6">
         <v>12</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="6">
         <v>13</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="6">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -877,6 +872,11 @@
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:M10"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cetak telaah penambahan tanda tangan
cetak telaah penambahan tanda tangan
</commit_message>
<xml_diff>
--- a/api/client/templates/cetak/laporan_pemeliharaan_telaah.xlsx
+++ b/api/client/templates/cetak/laporan_pemeliharaan_telaah.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>TAHUN 2024</t>
-  </si>
-  <si>
-    <t>HASIL PENELAAHAN RENCANA KEBUTUHAN PENGADAAN BARANG MILIK DAERAH</t>
-  </si>
-  <si>
-    <t>(RENCANA PENGADAAN)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>PEMERINTAH PROVINSI     : JAWA TENGAH</t>
   </si>
@@ -89,7 +80,13 @@
     <t>NAMA PEMELIHARAAN</t>
   </si>
   <si>
-    <t>PENGGUNA BARANG</t>
+    <t>(RENCANA PEMELIHARAAN)</t>
+  </si>
+  <si>
+    <t>PEMERINTAH KABUPATEN BANJARNEGARA</t>
+  </si>
+  <si>
+    <t>HASIL PENELAAHAN RENCANA PEMELIHARAAN BARANG MILIK DAERAH</t>
   </si>
 </sst>
 </file>
@@ -268,35 +265,35 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,7 +578,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:N4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,76 +592,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="A1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="A2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="A3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -683,11 +678,11 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="A6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -701,11 +696,11 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -719,9 +714,9 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -745,78 +740,78 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="14" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17" t="s">
+      <c r="C11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="10" t="s">
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="K11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="L11" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
@@ -864,6 +859,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:N4"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -872,11 +872,6 @@
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:M10"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:N4"/>
-    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>